<commit_message>
add backward command control
</commit_message>
<xml_diff>
--- a/outputs/tf/EfficientNetB0.xlsx
+++ b/outputs/tf/EfficientNetB0.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Details" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Details" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -27,7 +26,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -59,38 +63,62 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -121,9 +149,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -142,13 +170,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="0000FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="00FFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -514,9 +535,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA242"/>
+  <dimension ref="A1:X242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -528,7 +549,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr"/>
+      <c r="A1" s="10" t="n"/>
       <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Layer Hierarchy</t>
@@ -588,16 +609,9 @@
       </c>
       <c r="W1" s="12" t="n"/>
       <c r="X1" s="11" t="n"/>
-      <c r="Y1" s="10" t="inlineStr">
-        <is>
-          <t>Backward Ops</t>
-        </is>
-      </c>
-      <c r="Z1" s="12" t="n"/>
-      <c r="AA1" s="11" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr"/>
+      <c r="A2" s="10" t="n"/>
       <c r="B2" s="10" t="inlineStr">
         <is>
           <t>Layer</t>
@@ -709,21 +723,6 @@
         </is>
       </c>
       <c r="X2" s="10" t="inlineStr">
-        <is>
-          <t>Activation</t>
-        </is>
-      </c>
-      <c r="Y2" s="10" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
-      </c>
-      <c r="Z2" s="10" t="inlineStr">
-        <is>
-          <t>ElemWise</t>
-        </is>
-      </c>
-      <c r="AA2" s="10" t="inlineStr">
         <is>
           <t>Activation</t>
         </is>
@@ -780,9 +779,6 @@
       <c r="V3" s="8" t="n"/>
       <c r="W3" s="8" t="n"/>
       <c r="X3" s="8" t="n"/>
-      <c r="Y3" s="8" t="n"/>
-      <c r="Z3" s="8" t="n"/>
-      <c r="AA3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="n">
@@ -835,9 +831,6 @@
       <c r="V4" s="8" t="n"/>
       <c r="W4" s="8" t="n"/>
       <c r="X4" s="8" t="n"/>
-      <c r="Y4" s="8" t="n"/>
-      <c r="Z4" s="8" t="n"/>
-      <c r="AA4" s="8" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="n">
@@ -894,11 +887,6 @@
       </c>
       <c r="W5" s="8" t="n"/>
       <c r="X5" s="8" t="n"/>
-      <c r="Y5" s="8" t="n">
-        <v>7</v>
-      </c>
-      <c r="Z5" s="8" t="n"/>
-      <c r="AA5" s="8" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="7" t="n">
@@ -951,9 +939,6 @@
       <c r="V6" s="8" t="n"/>
       <c r="W6" s="8" t="n"/>
       <c r="X6" s="8" t="n"/>
-      <c r="Y6" s="8" t="n"/>
-      <c r="Z6" s="8" t="n"/>
-      <c r="AA6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="n">
@@ -1022,11 +1007,6 @@
       </c>
       <c r="W7" s="8" t="n"/>
       <c r="X7" s="8" t="n"/>
-      <c r="Y7" s="8" t="n">
-        <v>10838016</v>
-      </c>
-      <c r="Z7" s="8" t="n"/>
-      <c r="AA7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="n">
@@ -1083,11 +1063,6 @@
         <v>802816</v>
       </c>
       <c r="X8" s="8" t="n"/>
-      <c r="Y8" s="8" t="n"/>
-      <c r="Z8" s="8" t="n">
-        <v>802816</v>
-      </c>
-      <c r="AA8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="n">
@@ -1142,11 +1117,6 @@
       <c r="X9" s="8" t="n">
         <v>401408</v>
       </c>
-      <c r="Y9" s="8" t="n"/>
-      <c r="Z9" s="8" t="n"/>
-      <c r="AA9" s="8" t="n">
-        <v>401408</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="n">
@@ -1215,11 +1185,6 @@
       </c>
       <c r="W10" s="8" t="n"/>
       <c r="X10" s="8" t="n"/>
-      <c r="Y10" s="8" t="n">
-        <v>3612672</v>
-      </c>
-      <c r="Z10" s="8" t="n"/>
-      <c r="AA10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n">
@@ -1276,11 +1241,6 @@
         <v>802816</v>
       </c>
       <c r="X11" s="8" t="n"/>
-      <c r="Y11" s="8" t="n"/>
-      <c r="Z11" s="8" t="n">
-        <v>802816</v>
-      </c>
-      <c r="AA11" s="8" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="7" t="n">
@@ -1333,11 +1293,6 @@
       <c r="V12" s="8" t="n"/>
       <c r="W12" s="8" t="n"/>
       <c r="X12" s="8" t="n">
-        <v>401408</v>
-      </c>
-      <c r="Y12" s="8" t="n"/>
-      <c r="Z12" s="8" t="n"/>
-      <c r="AA12" s="8" t="n">
         <v>401408</v>
       </c>
     </row>
@@ -1390,11 +1345,6 @@
         <v>401376</v>
       </c>
       <c r="X13" s="8" t="n"/>
-      <c r="Y13" s="8" t="n"/>
-      <c r="Z13" s="8" t="n">
-        <v>401376</v>
-      </c>
-      <c r="AA13" s="8" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="7" t="n">
@@ -1443,9 +1393,6 @@
       <c r="V14" s="8" t="n"/>
       <c r="W14" s="8" t="n"/>
       <c r="X14" s="8" t="n"/>
-      <c r="Y14" s="8" t="n"/>
-      <c r="Z14" s="8" t="n"/>
-      <c r="AA14" s="8" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="7" t="n">
@@ -1514,11 +1461,6 @@
       </c>
       <c r="W15" s="8" t="n"/>
       <c r="X15" s="8" t="n"/>
-      <c r="Y15" s="8" t="n">
-        <v>264</v>
-      </c>
-      <c r="Z15" s="8" t="n"/>
-      <c r="AA15" s="8" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="7" t="n">
@@ -1587,11 +1529,6 @@
       </c>
       <c r="W16" s="8" t="n"/>
       <c r="X16" s="8" t="n"/>
-      <c r="Y16" s="8" t="n">
-        <v>288</v>
-      </c>
-      <c r="Z16" s="8" t="n"/>
-      <c r="AA16" s="8" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="7" t="n">
@@ -1650,9 +1587,6 @@
       <c r="V17" s="8" t="n"/>
       <c r="W17" s="8" t="n"/>
       <c r="X17" s="8" t="n"/>
-      <c r="Y17" s="8" t="n"/>
-      <c r="Z17" s="8" t="n"/>
-      <c r="AA17" s="8" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="7" t="n">
@@ -1721,11 +1655,6 @@
       </c>
       <c r="W18" s="8" t="n"/>
       <c r="X18" s="8" t="n"/>
-      <c r="Y18" s="8" t="n">
-        <v>6422528</v>
-      </c>
-      <c r="Z18" s="8" t="n"/>
-      <c r="AA18" s="8" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="7" t="n">
@@ -1782,11 +1711,6 @@
         <v>401408</v>
       </c>
       <c r="X19" s="8" t="n"/>
-      <c r="Y19" s="8" t="n"/>
-      <c r="Z19" s="8" t="n">
-        <v>401408</v>
-      </c>
-      <c r="AA19" s="8" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="7" t="n">
@@ -1855,11 +1779,6 @@
       </c>
       <c r="W20" s="8" t="n"/>
       <c r="X20" s="8" t="n"/>
-      <c r="Y20" s="8" t="n">
-        <v>19267584</v>
-      </c>
-      <c r="Z20" s="8" t="n"/>
-      <c r="AA20" s="8" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="7" t="n">
@@ -1916,11 +1835,6 @@
         <v>2408448</v>
       </c>
       <c r="X21" s="8" t="n"/>
-      <c r="Y21" s="8" t="n"/>
-      <c r="Z21" s="8" t="n">
-        <v>2408448</v>
-      </c>
-      <c r="AA21" s="8" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n">
@@ -1975,11 +1889,6 @@
       <c r="X22" s="8" t="n">
         <v>1204224</v>
       </c>
-      <c r="Y22" s="8" t="n"/>
-      <c r="Z22" s="8" t="n"/>
-      <c r="AA22" s="8" t="n">
-        <v>1204224</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="7" t="n">
@@ -2032,9 +1941,6 @@
       <c r="V23" s="8" t="n"/>
       <c r="W23" s="8" t="n"/>
       <c r="X23" s="8" t="n"/>
-      <c r="Y23" s="8" t="n"/>
-      <c r="Z23" s="8" t="n"/>
-      <c r="AA23" s="8" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="7" t="n">
@@ -2103,11 +2009,6 @@
       </c>
       <c r="W24" s="8" t="n"/>
       <c r="X24" s="8" t="n"/>
-      <c r="Y24" s="8" t="n">
-        <v>2709504</v>
-      </c>
-      <c r="Z24" s="8" t="n"/>
-      <c r="AA24" s="8" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="7" t="n">
@@ -2164,11 +2065,6 @@
         <v>602112</v>
       </c>
       <c r="X25" s="8" t="n"/>
-      <c r="Y25" s="8" t="n"/>
-      <c r="Z25" s="8" t="n">
-        <v>602112</v>
-      </c>
-      <c r="AA25" s="8" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="n">
@@ -2221,11 +2117,6 @@
       <c r="V26" s="8" t="n"/>
       <c r="W26" s="8" t="n"/>
       <c r="X26" s="8" t="n">
-        <v>301056</v>
-      </c>
-      <c r="Y26" s="8" t="n"/>
-      <c r="Z26" s="8" t="n"/>
-      <c r="AA26" s="8" t="n">
         <v>301056</v>
       </c>
     </row>
@@ -2278,11 +2169,6 @@
         <v>300960</v>
       </c>
       <c r="X27" s="8" t="n"/>
-      <c r="Y27" s="8" t="n"/>
-      <c r="Z27" s="8" t="n">
-        <v>300960</v>
-      </c>
-      <c r="AA27" s="8" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="7" t="n">
@@ -2331,9 +2217,6 @@
       <c r="V28" s="8" t="n"/>
       <c r="W28" s="8" t="n"/>
       <c r="X28" s="8" t="n"/>
-      <c r="Y28" s="8" t="n"/>
-      <c r="Z28" s="8" t="n"/>
-      <c r="AA28" s="8" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="7" t="n">
@@ -2402,11 +2285,6 @@
       </c>
       <c r="W29" s="8" t="n"/>
       <c r="X29" s="8" t="n"/>
-      <c r="Y29" s="8" t="n">
-        <v>388</v>
-      </c>
-      <c r="Z29" s="8" t="n"/>
-      <c r="AA29" s="8" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="7" t="n">
@@ -2475,11 +2353,6 @@
       </c>
       <c r="W30" s="8" t="n"/>
       <c r="X30" s="8" t="n"/>
-      <c r="Y30" s="8" t="n">
-        <v>480</v>
-      </c>
-      <c r="Z30" s="8" t="n"/>
-      <c r="AA30" s="8" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="7" t="n">
@@ -2538,9 +2411,6 @@
       <c r="V31" s="8" t="n"/>
       <c r="W31" s="8" t="n"/>
       <c r="X31" s="8" t="n"/>
-      <c r="Y31" s="8" t="n"/>
-      <c r="Z31" s="8" t="n"/>
-      <c r="AA31" s="8" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="7" t="n">
@@ -2609,11 +2479,6 @@
       </c>
       <c r="W32" s="8" t="n"/>
       <c r="X32" s="8" t="n"/>
-      <c r="Y32" s="8" t="n">
-        <v>7225344</v>
-      </c>
-      <c r="Z32" s="8" t="n"/>
-      <c r="AA32" s="8" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="7" t="n">
@@ -2670,11 +2535,6 @@
         <v>150528</v>
       </c>
       <c r="X33" s="8" t="n"/>
-      <c r="Y33" s="8" t="n"/>
-      <c r="Z33" s="8" t="n">
-        <v>150528</v>
-      </c>
-      <c r="AA33" s="8" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="7" t="n">
@@ -2743,11 +2603,6 @@
       </c>
       <c r="W34" s="8" t="n"/>
       <c r="X34" s="8" t="n"/>
-      <c r="Y34" s="8" t="n">
-        <v>10838016</v>
-      </c>
-      <c r="Z34" s="8" t="n"/>
-      <c r="AA34" s="8" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="7" t="n">
@@ -2804,11 +2659,6 @@
         <v>903168</v>
       </c>
       <c r="X35" s="8" t="n"/>
-      <c r="Y35" s="8" t="n"/>
-      <c r="Z35" s="8" t="n">
-        <v>903168</v>
-      </c>
-      <c r="AA35" s="8" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="7" t="n">
@@ -2863,11 +2713,6 @@
       <c r="X36" s="8" t="n">
         <v>451584</v>
       </c>
-      <c r="Y36" s="8" t="n"/>
-      <c r="Z36" s="8" t="n"/>
-      <c r="AA36" s="8" t="n">
-        <v>451584</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" s="7" t="n">
@@ -2936,11 +2781,6 @@
       </c>
       <c r="W37" s="8" t="n"/>
       <c r="X37" s="8" t="n"/>
-      <c r="Y37" s="8" t="n">
-        <v>4064256</v>
-      </c>
-      <c r="Z37" s="8" t="n"/>
-      <c r="AA37" s="8" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="7" t="n">
@@ -2997,11 +2837,6 @@
         <v>903168</v>
       </c>
       <c r="X38" s="8" t="n"/>
-      <c r="Y38" s="8" t="n"/>
-      <c r="Z38" s="8" t="n">
-        <v>903168</v>
-      </c>
-      <c r="AA38" s="8" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="7" t="n">
@@ -3054,11 +2889,6 @@
       <c r="V39" s="8" t="n"/>
       <c r="W39" s="8" t="n"/>
       <c r="X39" s="8" t="n">
-        <v>451584</v>
-      </c>
-      <c r="Y39" s="8" t="n"/>
-      <c r="Z39" s="8" t="n"/>
-      <c r="AA39" s="8" t="n">
         <v>451584</v>
       </c>
     </row>
@@ -3111,11 +2941,6 @@
         <v>451440</v>
       </c>
       <c r="X40" s="8" t="n"/>
-      <c r="Y40" s="8" t="n"/>
-      <c r="Z40" s="8" t="n">
-        <v>451440</v>
-      </c>
-      <c r="AA40" s="8" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="7" t="n">
@@ -3164,9 +2989,6 @@
       <c r="V41" s="8" t="n"/>
       <c r="W41" s="8" t="n"/>
       <c r="X41" s="8" t="n"/>
-      <c r="Y41" s="8" t="n"/>
-      <c r="Z41" s="8" t="n"/>
-      <c r="AA41" s="8" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="7" t="n">
@@ -3235,11 +3057,6 @@
       </c>
       <c r="W42" s="8" t="n"/>
       <c r="X42" s="8" t="n"/>
-      <c r="Y42" s="8" t="n">
-        <v>870</v>
-      </c>
-      <c r="Z42" s="8" t="n"/>
-      <c r="AA42" s="8" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="7" t="n">
@@ -3308,11 +3125,6 @@
       </c>
       <c r="W43" s="8" t="n"/>
       <c r="X43" s="8" t="n"/>
-      <c r="Y43" s="8" t="n">
-        <v>1008</v>
-      </c>
-      <c r="Z43" s="8" t="n"/>
-      <c r="AA43" s="8" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="7" t="n">
@@ -3371,9 +3183,6 @@
       <c r="V44" s="8" t="n"/>
       <c r="W44" s="8" t="n"/>
       <c r="X44" s="8" t="n"/>
-      <c r="Y44" s="8" t="n"/>
-      <c r="Z44" s="8" t="n"/>
-      <c r="AA44" s="8" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="7" t="n">
@@ -3442,11 +3251,6 @@
       </c>
       <c r="W45" s="8" t="n"/>
       <c r="X45" s="8" t="n"/>
-      <c r="Y45" s="8" t="n">
-        <v>10838016</v>
-      </c>
-      <c r="Z45" s="8" t="n"/>
-      <c r="AA45" s="8" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="7" t="n">
@@ -3503,11 +3307,6 @@
         <v>150528</v>
       </c>
       <c r="X46" s="8" t="n"/>
-      <c r="Y46" s="8" t="n"/>
-      <c r="Z46" s="8" t="n">
-        <v>150528</v>
-      </c>
-      <c r="AA46" s="8" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="7" t="n">
@@ -3560,9 +3359,6 @@
       <c r="V47" s="8" t="n"/>
       <c r="W47" s="8" t="n"/>
       <c r="X47" s="8" t="n"/>
-      <c r="Y47" s="8" t="n"/>
-      <c r="Z47" s="8" t="n"/>
-      <c r="AA47" s="8" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="7" t="n">
@@ -3623,11 +3419,6 @@
         <v>75264</v>
       </c>
       <c r="X48" s="8" t="n"/>
-      <c r="Y48" s="8" t="n"/>
-      <c r="Z48" s="8" t="n">
-        <v>75264</v>
-      </c>
-      <c r="AA48" s="8" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="7" t="n">
@@ -3696,11 +3487,6 @@
       </c>
       <c r="W49" s="8" t="n"/>
       <c r="X49" s="8" t="n"/>
-      <c r="Y49" s="8" t="n">
-        <v>10838016</v>
-      </c>
-      <c r="Z49" s="8" t="n"/>
-      <c r="AA49" s="8" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="7" t="n">
@@ -3757,11 +3543,6 @@
         <v>903168</v>
       </c>
       <c r="X50" s="8" t="n"/>
-      <c r="Y50" s="8" t="n"/>
-      <c r="Z50" s="8" t="n">
-        <v>903168</v>
-      </c>
-      <c r="AA50" s="8" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="7" t="n">
@@ -3816,11 +3597,6 @@
       <c r="X51" s="8" t="n">
         <v>451584</v>
       </c>
-      <c r="Y51" s="8" t="n"/>
-      <c r="Z51" s="8" t="n"/>
-      <c r="AA51" s="8" t="n">
-        <v>451584</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" s="7" t="n">
@@ -3873,9 +3649,6 @@
       <c r="V52" s="8" t="n"/>
       <c r="W52" s="8" t="n"/>
       <c r="X52" s="8" t="n"/>
-      <c r="Y52" s="8" t="n"/>
-      <c r="Z52" s="8" t="n"/>
-      <c r="AA52" s="8" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="7" t="n">
@@ -3944,11 +3717,6 @@
       </c>
       <c r="W53" s="8" t="n"/>
       <c r="X53" s="8" t="n"/>
-      <c r="Y53" s="8" t="n">
-        <v>2822400</v>
-      </c>
-      <c r="Z53" s="8" t="n"/>
-      <c r="AA53" s="8" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="7" t="n">
@@ -4005,11 +3773,6 @@
         <v>225792</v>
       </c>
       <c r="X54" s="8" t="n"/>
-      <c r="Y54" s="8" t="n"/>
-      <c r="Z54" s="8" t="n">
-        <v>225792</v>
-      </c>
-      <c r="AA54" s="8" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="7" t="n">
@@ -4062,11 +3825,6 @@
       <c r="V55" s="8" t="n"/>
       <c r="W55" s="8" t="n"/>
       <c r="X55" s="8" t="n">
-        <v>112896</v>
-      </c>
-      <c r="Y55" s="8" t="n"/>
-      <c r="Z55" s="8" t="n"/>
-      <c r="AA55" s="8" t="n">
         <v>112896</v>
       </c>
     </row>
@@ -4119,11 +3877,6 @@
         <v>112752</v>
       </c>
       <c r="X56" s="8" t="n"/>
-      <c r="Y56" s="8" t="n"/>
-      <c r="Z56" s="8" t="n">
-        <v>112752</v>
-      </c>
-      <c r="AA56" s="8" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="7" t="n">
@@ -4172,9 +3925,6 @@
       <c r="V57" s="8" t="n"/>
       <c r="W57" s="8" t="n"/>
       <c r="X57" s="8" t="n"/>
-      <c r="Y57" s="8" t="n"/>
-      <c r="Z57" s="8" t="n"/>
-      <c r="AA57" s="8" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="7" t="n">
@@ -4243,11 +3993,6 @@
       </c>
       <c r="W58" s="8" t="n"/>
       <c r="X58" s="8" t="n"/>
-      <c r="Y58" s="8" t="n">
-        <v>870</v>
-      </c>
-      <c r="Z58" s="8" t="n"/>
-      <c r="AA58" s="8" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="7" t="n">
@@ -4316,11 +4061,6 @@
       </c>
       <c r="W59" s="8" t="n"/>
       <c r="X59" s="8" t="n"/>
-      <c r="Y59" s="8" t="n">
-        <v>1008</v>
-      </c>
-      <c r="Z59" s="8" t="n"/>
-      <c r="AA59" s="8" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="7" t="n">
@@ -4379,9 +4119,6 @@
       <c r="V60" s="8" t="n"/>
       <c r="W60" s="8" t="n"/>
       <c r="X60" s="8" t="n"/>
-      <c r="Y60" s="8" t="n"/>
-      <c r="Z60" s="8" t="n"/>
-      <c r="AA60" s="8" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="7" t="n">
@@ -4450,11 +4187,6 @@
       </c>
       <c r="W61" s="8" t="n"/>
       <c r="X61" s="8" t="n"/>
-      <c r="Y61" s="8" t="n">
-        <v>4515840</v>
-      </c>
-      <c r="Z61" s="8" t="n"/>
-      <c r="AA61" s="8" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="7" t="n">
@@ -4511,11 +4243,6 @@
         <v>62720</v>
       </c>
       <c r="X62" s="8" t="n"/>
-      <c r="Y62" s="8" t="n"/>
-      <c r="Z62" s="8" t="n">
-        <v>62720</v>
-      </c>
-      <c r="AA62" s="8" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="7" t="n">
@@ -4584,11 +4311,6 @@
       </c>
       <c r="W63" s="8" t="n"/>
       <c r="X63" s="8" t="n"/>
-      <c r="Y63" s="8" t="n">
-        <v>7526400</v>
-      </c>
-      <c r="Z63" s="8" t="n"/>
-      <c r="AA63" s="8" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="7" t="n">
@@ -4645,11 +4367,6 @@
         <v>376320</v>
       </c>
       <c r="X64" s="8" t="n"/>
-      <c r="Y64" s="8" t="n"/>
-      <c r="Z64" s="8" t="n">
-        <v>376320</v>
-      </c>
-      <c r="AA64" s="8" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="7" t="n">
@@ -4704,11 +4421,6 @@
       <c r="X65" s="8" t="n">
         <v>188160</v>
       </c>
-      <c r="Y65" s="8" t="n"/>
-      <c r="Z65" s="8" t="n"/>
-      <c r="AA65" s="8" t="n">
-        <v>188160</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" s="7" t="n">
@@ -4777,11 +4489,6 @@
       </c>
       <c r="W66" s="8" t="n"/>
       <c r="X66" s="8" t="n"/>
-      <c r="Y66" s="8" t="n">
-        <v>4704000</v>
-      </c>
-      <c r="Z66" s="8" t="n"/>
-      <c r="AA66" s="8" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="7" t="n">
@@ -4838,11 +4545,6 @@
         <v>376320</v>
       </c>
       <c r="X67" s="8" t="n"/>
-      <c r="Y67" s="8" t="n"/>
-      <c r="Z67" s="8" t="n">
-        <v>376320</v>
-      </c>
-      <c r="AA67" s="8" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="7" t="n">
@@ -4895,11 +4597,6 @@
       <c r="V68" s="8" t="n"/>
       <c r="W68" s="8" t="n"/>
       <c r="X68" s="8" t="n">
-        <v>188160</v>
-      </c>
-      <c r="Y68" s="8" t="n"/>
-      <c r="Z68" s="8" t="n"/>
-      <c r="AA68" s="8" t="n">
         <v>188160</v>
       </c>
     </row>
@@ -4952,11 +4649,6 @@
         <v>187920</v>
       </c>
       <c r="X69" s="8" t="n"/>
-      <c r="Y69" s="8" t="n"/>
-      <c r="Z69" s="8" t="n">
-        <v>187920</v>
-      </c>
-      <c r="AA69" s="8" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="7" t="n">
@@ -5005,9 +4697,6 @@
       <c r="V70" s="8" t="n"/>
       <c r="W70" s="8" t="n"/>
       <c r="X70" s="8" t="n"/>
-      <c r="Y70" s="8" t="n"/>
-      <c r="Z70" s="8" t="n"/>
-      <c r="AA70" s="8" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="7" t="n">
@@ -5076,11 +4765,6 @@
       </c>
       <c r="W71" s="8" t="n"/>
       <c r="X71" s="8" t="n"/>
-      <c r="Y71" s="8" t="n">
-        <v>2410</v>
-      </c>
-      <c r="Z71" s="8" t="n"/>
-      <c r="AA71" s="8" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="7" t="n">
@@ -5149,11 +4833,6 @@
       </c>
       <c r="W72" s="8" t="n"/>
       <c r="X72" s="8" t="n"/>
-      <c r="Y72" s="8" t="n">
-        <v>2640</v>
-      </c>
-      <c r="Z72" s="8" t="n"/>
-      <c r="AA72" s="8" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="7" t="n">
@@ -5212,9 +4891,6 @@
       <c r="V73" s="8" t="n"/>
       <c r="W73" s="8" t="n"/>
       <c r="X73" s="8" t="n"/>
-      <c r="Y73" s="8" t="n"/>
-      <c r="Z73" s="8" t="n"/>
-      <c r="AA73" s="8" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="7" t="n">
@@ -5283,11 +4959,6 @@
       </c>
       <c r="W74" s="8" t="n"/>
       <c r="X74" s="8" t="n"/>
-      <c r="Y74" s="8" t="n">
-        <v>7526400</v>
-      </c>
-      <c r="Z74" s="8" t="n"/>
-      <c r="AA74" s="8" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="7" t="n">
@@ -5344,11 +5015,6 @@
         <v>62720</v>
       </c>
       <c r="X75" s="8" t="n"/>
-      <c r="Y75" s="8" t="n"/>
-      <c r="Z75" s="8" t="n">
-        <v>62720</v>
-      </c>
-      <c r="AA75" s="8" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="7" t="n">
@@ -5401,9 +5067,6 @@
       <c r="V76" s="8" t="n"/>
       <c r="W76" s="8" t="n"/>
       <c r="X76" s="8" t="n"/>
-      <c r="Y76" s="8" t="n"/>
-      <c r="Z76" s="8" t="n"/>
-      <c r="AA76" s="8" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="7" t="n">
@@ -5464,11 +5127,6 @@
         <v>31360</v>
       </c>
       <c r="X77" s="8" t="n"/>
-      <c r="Y77" s="8" t="n"/>
-      <c r="Z77" s="8" t="n">
-        <v>31360</v>
-      </c>
-      <c r="AA77" s="8" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="7" t="n">
@@ -5537,11 +5195,6 @@
       </c>
       <c r="W78" s="8" t="n"/>
       <c r="X78" s="8" t="n"/>
-      <c r="Y78" s="8" t="n">
-        <v>7526400</v>
-      </c>
-      <c r="Z78" s="8" t="n"/>
-      <c r="AA78" s="8" t="n"/>
     </row>
     <row r="79">
       <c r="A79" s="7" t="n">
@@ -5598,11 +5251,6 @@
         <v>376320</v>
       </c>
       <c r="X79" s="8" t="n"/>
-      <c r="Y79" s="8" t="n"/>
-      <c r="Z79" s="8" t="n">
-        <v>376320</v>
-      </c>
-      <c r="AA79" s="8" t="n"/>
     </row>
     <row r="80">
       <c r="A80" s="7" t="n">
@@ -5657,11 +5305,6 @@
       <c r="X80" s="8" t="n">
         <v>188160</v>
       </c>
-      <c r="Y80" s="8" t="n"/>
-      <c r="Z80" s="8" t="n"/>
-      <c r="AA80" s="8" t="n">
-        <v>188160</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" s="7" t="n">
@@ -5714,9 +5357,6 @@
       <c r="V81" s="8" t="n"/>
       <c r="W81" s="8" t="n"/>
       <c r="X81" s="8" t="n"/>
-      <c r="Y81" s="8" t="n"/>
-      <c r="Z81" s="8" t="n"/>
-      <c r="AA81" s="8" t="n"/>
     </row>
     <row r="82">
       <c r="A82" s="7" t="n">
@@ -5785,11 +5425,6 @@
       </c>
       <c r="W82" s="8" t="n"/>
       <c r="X82" s="8" t="n"/>
-      <c r="Y82" s="8" t="n">
-        <v>423360</v>
-      </c>
-      <c r="Z82" s="8" t="n"/>
-      <c r="AA82" s="8" t="n"/>
     </row>
     <row r="83">
       <c r="A83" s="7" t="n">
@@ -5846,11 +5481,6 @@
         <v>94080</v>
       </c>
       <c r="X83" s="8" t="n"/>
-      <c r="Y83" s="8" t="n"/>
-      <c r="Z83" s="8" t="n">
-        <v>94080</v>
-      </c>
-      <c r="AA83" s="8" t="n"/>
     </row>
     <row r="84">
       <c r="A84" s="7" t="n">
@@ -5903,11 +5533,6 @@
       <c r="V84" s="8" t="n"/>
       <c r="W84" s="8" t="n"/>
       <c r="X84" s="8" t="n">
-        <v>47040</v>
-      </c>
-      <c r="Y84" s="8" t="n"/>
-      <c r="Z84" s="8" t="n"/>
-      <c r="AA84" s="8" t="n">
         <v>47040</v>
       </c>
     </row>
@@ -5960,11 +5585,6 @@
         <v>46800</v>
       </c>
       <c r="X85" s="8" t="n"/>
-      <c r="Y85" s="8" t="n"/>
-      <c r="Z85" s="8" t="n">
-        <v>46800</v>
-      </c>
-      <c r="AA85" s="8" t="n"/>
     </row>
     <row r="86">
       <c r="A86" s="7" t="n">
@@ -6013,9 +5633,6 @@
       <c r="V86" s="8" t="n"/>
       <c r="W86" s="8" t="n"/>
       <c r="X86" s="8" t="n"/>
-      <c r="Y86" s="8" t="n"/>
-      <c r="Z86" s="8" t="n"/>
-      <c r="AA86" s="8" t="n"/>
     </row>
     <row r="87">
       <c r="A87" s="7" t="n">
@@ -6084,11 +5701,6 @@
       </c>
       <c r="W87" s="8" t="n"/>
       <c r="X87" s="8" t="n"/>
-      <c r="Y87" s="8" t="n">
-        <v>2410</v>
-      </c>
-      <c r="Z87" s="8" t="n"/>
-      <c r="AA87" s="8" t="n"/>
     </row>
     <row r="88">
       <c r="A88" s="7" t="n">
@@ -6157,11 +5769,6 @@
       </c>
       <c r="W88" s="8" t="n"/>
       <c r="X88" s="8" t="n"/>
-      <c r="Y88" s="8" t="n">
-        <v>2640</v>
-      </c>
-      <c r="Z88" s="8" t="n"/>
-      <c r="AA88" s="8" t="n"/>
     </row>
     <row r="89">
       <c r="A89" s="7" t="n">
@@ -6220,9 +5827,6 @@
       <c r="V89" s="8" t="n"/>
       <c r="W89" s="8" t="n"/>
       <c r="X89" s="8" t="n"/>
-      <c r="Y89" s="8" t="n"/>
-      <c r="Z89" s="8" t="n"/>
-      <c r="AA89" s="8" t="n"/>
     </row>
     <row r="90">
       <c r="A90" s="7" t="n">
@@ -6291,11 +5895,6 @@
       </c>
       <c r="W90" s="8" t="n"/>
       <c r="X90" s="8" t="n"/>
-      <c r="Y90" s="8" t="n">
-        <v>3763200</v>
-      </c>
-      <c r="Z90" s="8" t="n"/>
-      <c r="AA90" s="8" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="7" t="n">
@@ -6352,11 +5951,6 @@
         <v>31360</v>
       </c>
       <c r="X91" s="8" t="n"/>
-      <c r="Y91" s="8" t="n"/>
-      <c r="Z91" s="8" t="n">
-        <v>31360</v>
-      </c>
-      <c r="AA91" s="8" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="7" t="n">
@@ -6425,11 +6019,6 @@
       </c>
       <c r="W92" s="8" t="n"/>
       <c r="X92" s="8" t="n"/>
-      <c r="Y92" s="8" t="n">
-        <v>7526400</v>
-      </c>
-      <c r="Z92" s="8" t="n"/>
-      <c r="AA92" s="8" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="7" t="n">
@@ -6486,11 +6075,6 @@
         <v>188160</v>
       </c>
       <c r="X93" s="8" t="n"/>
-      <c r="Y93" s="8" t="n"/>
-      <c r="Z93" s="8" t="n">
-        <v>188160</v>
-      </c>
-      <c r="AA93" s="8" t="n"/>
     </row>
     <row r="94">
       <c r="A94" s="7" t="n">
@@ -6545,11 +6129,6 @@
       <c r="X94" s="8" t="n">
         <v>94080</v>
       </c>
-      <c r="Y94" s="8" t="n"/>
-      <c r="Z94" s="8" t="n"/>
-      <c r="AA94" s="8" t="n">
-        <v>94080</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" s="7" t="n">
@@ -6618,11 +6197,6 @@
       </c>
       <c r="W95" s="8" t="n"/>
       <c r="X95" s="8" t="n"/>
-      <c r="Y95" s="8" t="n">
-        <v>846720</v>
-      </c>
-      <c r="Z95" s="8" t="n"/>
-      <c r="AA95" s="8" t="n"/>
     </row>
     <row r="96">
       <c r="A96" s="7" t="n">
@@ -6679,11 +6253,6 @@
         <v>188160</v>
       </c>
       <c r="X96" s="8" t="n"/>
-      <c r="Y96" s="8" t="n"/>
-      <c r="Z96" s="8" t="n">
-        <v>188160</v>
-      </c>
-      <c r="AA96" s="8" t="n"/>
     </row>
     <row r="97">
       <c r="A97" s="7" t="n">
@@ -6736,11 +6305,6 @@
       <c r="V97" s="8" t="n"/>
       <c r="W97" s="8" t="n"/>
       <c r="X97" s="8" t="n">
-        <v>94080</v>
-      </c>
-      <c r="Y97" s="8" t="n"/>
-      <c r="Z97" s="8" t="n"/>
-      <c r="AA97" s="8" t="n">
         <v>94080</v>
       </c>
     </row>
@@ -6793,11 +6357,6 @@
         <v>93600</v>
       </c>
       <c r="X98" s="8" t="n"/>
-      <c r="Y98" s="8" t="n"/>
-      <c r="Z98" s="8" t="n">
-        <v>93600</v>
-      </c>
-      <c r="AA98" s="8" t="n"/>
     </row>
     <row r="99">
       <c r="A99" s="7" t="n">
@@ -6846,9 +6405,6 @@
       <c r="V99" s="8" t="n"/>
       <c r="W99" s="8" t="n"/>
       <c r="X99" s="8" t="n"/>
-      <c r="Y99" s="8" t="n"/>
-      <c r="Z99" s="8" t="n"/>
-      <c r="AA99" s="8" t="n"/>
     </row>
     <row r="100">
       <c r="A100" s="7" t="n">
@@ -6917,11 +6473,6 @@
       </c>
       <c r="W100" s="8" t="n"/>
       <c r="X100" s="8" t="n"/>
-      <c r="Y100" s="8" t="n">
-        <v>9620</v>
-      </c>
-      <c r="Z100" s="8" t="n"/>
-      <c r="AA100" s="8" t="n"/>
     </row>
     <row r="101">
       <c r="A101" s="7" t="n">
@@ -6990,11 +6541,6 @@
       </c>
       <c r="W101" s="8" t="n"/>
       <c r="X101" s="8" t="n"/>
-      <c r="Y101" s="8" t="n">
-        <v>10080</v>
-      </c>
-      <c r="Z101" s="8" t="n"/>
-      <c r="AA101" s="8" t="n"/>
     </row>
     <row r="102">
       <c r="A102" s="7" t="n">
@@ -7053,9 +6599,6 @@
       <c r="V102" s="8" t="n"/>
       <c r="W102" s="8" t="n"/>
       <c r="X102" s="8" t="n"/>
-      <c r="Y102" s="8" t="n"/>
-      <c r="Z102" s="8" t="n"/>
-      <c r="AA102" s="8" t="n"/>
     </row>
     <row r="103">
       <c r="A103" s="7" t="n">
@@ -7124,11 +6667,6 @@
       </c>
       <c r="W103" s="8" t="n"/>
       <c r="X103" s="8" t="n"/>
-      <c r="Y103" s="8" t="n">
-        <v>7526400</v>
-      </c>
-      <c r="Z103" s="8" t="n"/>
-      <c r="AA103" s="8" t="n"/>
     </row>
     <row r="104">
       <c r="A104" s="7" t="n">
@@ -7185,11 +6723,6 @@
         <v>31360</v>
       </c>
       <c r="X104" s="8" t="n"/>
-      <c r="Y104" s="8" t="n"/>
-      <c r="Z104" s="8" t="n">
-        <v>31360</v>
-      </c>
-      <c r="AA104" s="8" t="n"/>
     </row>
     <row r="105">
       <c r="A105" s="7" t="n">
@@ -7242,9 +6775,6 @@
       <c r="V105" s="8" t="n"/>
       <c r="W105" s="8" t="n"/>
       <c r="X105" s="8" t="n"/>
-      <c r="Y105" s="8" t="n"/>
-      <c r="Z105" s="8" t="n"/>
-      <c r="AA105" s="8" t="n"/>
     </row>
     <row r="106">
       <c r="A106" s="7" t="n">
@@ -7305,11 +6835,6 @@
         <v>15680</v>
       </c>
       <c r="X106" s="8" t="n"/>
-      <c r="Y106" s="8" t="n"/>
-      <c r="Z106" s="8" t="n">
-        <v>15680</v>
-      </c>
-      <c r="AA106" s="8" t="n"/>
     </row>
     <row r="107">
       <c r="A107" s="7" t="n">
@@ -7378,11 +6903,6 @@
       </c>
       <c r="W107" s="8" t="n"/>
       <c r="X107" s="8" t="n"/>
-      <c r="Y107" s="8" t="n">
-        <v>7526400</v>
-      </c>
-      <c r="Z107" s="8" t="n"/>
-      <c r="AA107" s="8" t="n"/>
     </row>
     <row r="108">
       <c r="A108" s="7" t="n">
@@ -7439,11 +6959,6 @@
         <v>188160</v>
       </c>
       <c r="X108" s="8" t="n"/>
-      <c r="Y108" s="8" t="n"/>
-      <c r="Z108" s="8" t="n">
-        <v>188160</v>
-      </c>
-      <c r="AA108" s="8" t="n"/>
     </row>
     <row r="109">
       <c r="A109" s="7" t="n">
@@ -7498,11 +7013,6 @@
       <c r="X109" s="8" t="n">
         <v>94080</v>
       </c>
-      <c r="Y109" s="8" t="n"/>
-      <c r="Z109" s="8" t="n"/>
-      <c r="AA109" s="8" t="n">
-        <v>94080</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" s="7" t="n">
@@ -7571,11 +7081,6 @@
       </c>
       <c r="W110" s="8" t="n"/>
       <c r="X110" s="8" t="n"/>
-      <c r="Y110" s="8" t="n">
-        <v>846720</v>
-      </c>
-      <c r="Z110" s="8" t="n"/>
-      <c r="AA110" s="8" t="n"/>
     </row>
     <row r="111">
       <c r="A111" s="7" t="n">
@@ -7632,11 +7137,6 @@
         <v>188160</v>
       </c>
       <c r="X111" s="8" t="n"/>
-      <c r="Y111" s="8" t="n"/>
-      <c r="Z111" s="8" t="n">
-        <v>188160</v>
-      </c>
-      <c r="AA111" s="8" t="n"/>
     </row>
     <row r="112">
       <c r="A112" s="7" t="n">
@@ -7689,11 +7189,6 @@
       <c r="V112" s="8" t="n"/>
       <c r="W112" s="8" t="n"/>
       <c r="X112" s="8" t="n">
-        <v>94080</v>
-      </c>
-      <c r="Y112" s="8" t="n"/>
-      <c r="Z112" s="8" t="n"/>
-      <c r="AA112" s="8" t="n">
         <v>94080</v>
       </c>
     </row>
@@ -7746,11 +7241,6 @@
         <v>93600</v>
       </c>
       <c r="X113" s="8" t="n"/>
-      <c r="Y113" s="8" t="n"/>
-      <c r="Z113" s="8" t="n">
-        <v>93600</v>
-      </c>
-      <c r="AA113" s="8" t="n"/>
     </row>
     <row r="114">
       <c r="A114" s="7" t="n">
@@ -7799,9 +7289,6 @@
       <c r="V114" s="8" t="n"/>
       <c r="W114" s="8" t="n"/>
       <c r="X114" s="8" t="n"/>
-      <c r="Y114" s="8" t="n"/>
-      <c r="Z114" s="8" t="n"/>
-      <c r="AA114" s="8" t="n"/>
     </row>
     <row r="115">
       <c r="A115" s="7" t="n">
@@ -7870,11 +7357,6 @@
       </c>
       <c r="W115" s="8" t="n"/>
       <c r="X115" s="8" t="n"/>
-      <c r="Y115" s="8" t="n">
-        <v>9620</v>
-      </c>
-      <c r="Z115" s="8" t="n"/>
-      <c r="AA115" s="8" t="n"/>
     </row>
     <row r="116">
       <c r="A116" s="7" t="n">
@@ -7943,11 +7425,6 @@
       </c>
       <c r="W116" s="8" t="n"/>
       <c r="X116" s="8" t="n"/>
-      <c r="Y116" s="8" t="n">
-        <v>10080</v>
-      </c>
-      <c r="Z116" s="8" t="n"/>
-      <c r="AA116" s="8" t="n"/>
     </row>
     <row r="117">
       <c r="A117" s="7" t="n">
@@ -8006,9 +7483,6 @@
       <c r="V117" s="8" t="n"/>
       <c r="W117" s="8" t="n"/>
       <c r="X117" s="8" t="n"/>
-      <c r="Y117" s="8" t="n"/>
-      <c r="Z117" s="8" t="n"/>
-      <c r="AA117" s="8" t="n"/>
     </row>
     <row r="118">
       <c r="A118" s="7" t="n">
@@ -8077,11 +7551,6 @@
       </c>
       <c r="W118" s="8" t="n"/>
       <c r="X118" s="8" t="n"/>
-      <c r="Y118" s="8" t="n">
-        <v>7526400</v>
-      </c>
-      <c r="Z118" s="8" t="n"/>
-      <c r="AA118" s="8" t="n"/>
     </row>
     <row r="119">
       <c r="A119" s="7" t="n">
@@ -8138,11 +7607,6 @@
         <v>31360</v>
       </c>
       <c r="X119" s="8" t="n"/>
-      <c r="Y119" s="8" t="n"/>
-      <c r="Z119" s="8" t="n">
-        <v>31360</v>
-      </c>
-      <c r="AA119" s="8" t="n"/>
     </row>
     <row r="120">
       <c r="A120" s="7" t="n">
@@ -8195,9 +7659,6 @@
       <c r="V120" s="8" t="n"/>
       <c r="W120" s="8" t="n"/>
       <c r="X120" s="8" t="n"/>
-      <c r="Y120" s="8" t="n"/>
-      <c r="Z120" s="8" t="n"/>
-      <c r="AA120" s="8" t="n"/>
     </row>
     <row r="121">
       <c r="A121" s="7" t="n">
@@ -8258,11 +7719,6 @@
         <v>15680</v>
       </c>
       <c r="X121" s="8" t="n"/>
-      <c r="Y121" s="8" t="n"/>
-      <c r="Z121" s="8" t="n">
-        <v>15680</v>
-      </c>
-      <c r="AA121" s="8" t="n"/>
     </row>
     <row r="122">
       <c r="A122" s="7" t="n">
@@ -8331,11 +7787,6 @@
       </c>
       <c r="W122" s="8" t="n"/>
       <c r="X122" s="8" t="n"/>
-      <c r="Y122" s="8" t="n">
-        <v>7526400</v>
-      </c>
-      <c r="Z122" s="8" t="n"/>
-      <c r="AA122" s="8" t="n"/>
     </row>
     <row r="123">
       <c r="A123" s="7" t="n">
@@ -8392,11 +7843,6 @@
         <v>188160</v>
       </c>
       <c r="X123" s="8" t="n"/>
-      <c r="Y123" s="8" t="n"/>
-      <c r="Z123" s="8" t="n">
-        <v>188160</v>
-      </c>
-      <c r="AA123" s="8" t="n"/>
     </row>
     <row r="124">
       <c r="A124" s="7" t="n">
@@ -8451,11 +7897,6 @@
       <c r="X124" s="8" t="n">
         <v>94080</v>
       </c>
-      <c r="Y124" s="8" t="n"/>
-      <c r="Z124" s="8" t="n"/>
-      <c r="AA124" s="8" t="n">
-        <v>94080</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" s="7" t="n">
@@ -8524,11 +7965,6 @@
       </c>
       <c r="W125" s="8" t="n"/>
       <c r="X125" s="8" t="n"/>
-      <c r="Y125" s="8" t="n">
-        <v>2352000</v>
-      </c>
-      <c r="Z125" s="8" t="n"/>
-      <c r="AA125" s="8" t="n"/>
     </row>
     <row r="126">
       <c r="A126" s="7" t="n">
@@ -8585,11 +8021,6 @@
         <v>188160</v>
       </c>
       <c r="X126" s="8" t="n"/>
-      <c r="Y126" s="8" t="n"/>
-      <c r="Z126" s="8" t="n">
-        <v>188160</v>
-      </c>
-      <c r="AA126" s="8" t="n"/>
     </row>
     <row r="127">
       <c r="A127" s="7" t="n">
@@ -8642,11 +8073,6 @@
       <c r="V127" s="8" t="n"/>
       <c r="W127" s="8" t="n"/>
       <c r="X127" s="8" t="n">
-        <v>94080</v>
-      </c>
-      <c r="Y127" s="8" t="n"/>
-      <c r="Z127" s="8" t="n"/>
-      <c r="AA127" s="8" t="n">
         <v>94080</v>
       </c>
     </row>
@@ -8699,11 +8125,6 @@
         <v>93600</v>
       </c>
       <c r="X128" s="8" t="n"/>
-      <c r="Y128" s="8" t="n"/>
-      <c r="Z128" s="8" t="n">
-        <v>93600</v>
-      </c>
-      <c r="AA128" s="8" t="n"/>
     </row>
     <row r="129">
       <c r="A129" s="7" t="n">
@@ -8752,9 +8173,6 @@
       <c r="V129" s="8" t="n"/>
       <c r="W129" s="8" t="n"/>
       <c r="X129" s="8" t="n"/>
-      <c r="Y129" s="8" t="n"/>
-      <c r="Z129" s="8" t="n"/>
-      <c r="AA129" s="8" t="n"/>
     </row>
     <row r="130">
       <c r="A130" s="7" t="n">
@@ -8823,11 +8241,6 @@
       </c>
       <c r="W130" s="8" t="n"/>
       <c r="X130" s="8" t="n"/>
-      <c r="Y130" s="8" t="n">
-        <v>9620</v>
-      </c>
-      <c r="Z130" s="8" t="n"/>
-      <c r="AA130" s="8" t="n"/>
     </row>
     <row r="131">
       <c r="A131" s="7" t="n">
@@ -8896,11 +8309,6 @@
       </c>
       <c r="W131" s="8" t="n"/>
       <c r="X131" s="8" t="n"/>
-      <c r="Y131" s="8" t="n">
-        <v>10080</v>
-      </c>
-      <c r="Z131" s="8" t="n"/>
-      <c r="AA131" s="8" t="n"/>
     </row>
     <row r="132">
       <c r="A132" s="7" t="n">
@@ -8959,9 +8367,6 @@
       <c r="V132" s="8" t="n"/>
       <c r="W132" s="8" t="n"/>
       <c r="X132" s="8" t="n"/>
-      <c r="Y132" s="8" t="n"/>
-      <c r="Z132" s="8" t="n"/>
-      <c r="AA132" s="8" t="n"/>
     </row>
     <row r="133">
       <c r="A133" s="7" t="n">
@@ -9030,11 +8435,6 @@
       </c>
       <c r="W133" s="8" t="n"/>
       <c r="X133" s="8" t="n"/>
-      <c r="Y133" s="8" t="n">
-        <v>10536960</v>
-      </c>
-      <c r="Z133" s="8" t="n"/>
-      <c r="AA133" s="8" t="n"/>
     </row>
     <row r="134">
       <c r="A134" s="7" t="n">
@@ -9091,11 +8491,6 @@
         <v>43904</v>
       </c>
       <c r="X134" s="8" t="n"/>
-      <c r="Y134" s="8" t="n"/>
-      <c r="Z134" s="8" t="n">
-        <v>43904</v>
-      </c>
-      <c r="AA134" s="8" t="n"/>
     </row>
     <row r="135">
       <c r="A135" s="7" t="n">
@@ -9164,11 +8559,6 @@
       </c>
       <c r="W135" s="8" t="n"/>
       <c r="X135" s="8" t="n"/>
-      <c r="Y135" s="8" t="n">
-        <v>14751744</v>
-      </c>
-      <c r="Z135" s="8" t="n"/>
-      <c r="AA135" s="8" t="n"/>
     </row>
     <row r="136">
       <c r="A136" s="7" t="n">
@@ -9225,11 +8615,6 @@
         <v>263424</v>
       </c>
       <c r="X136" s="8" t="n"/>
-      <c r="Y136" s="8" t="n"/>
-      <c r="Z136" s="8" t="n">
-        <v>263424</v>
-      </c>
-      <c r="AA136" s="8" t="n"/>
     </row>
     <row r="137">
       <c r="A137" s="7" t="n">
@@ -9284,11 +8669,6 @@
       <c r="X137" s="8" t="n">
         <v>131712</v>
       </c>
-      <c r="Y137" s="8" t="n"/>
-      <c r="Z137" s="8" t="n"/>
-      <c r="AA137" s="8" t="n">
-        <v>131712</v>
-      </c>
     </row>
     <row r="138">
       <c r="A138" s="7" t="n">
@@ -9357,11 +8737,6 @@
       </c>
       <c r="W138" s="8" t="n"/>
       <c r="X138" s="8" t="n"/>
-      <c r="Y138" s="8" t="n">
-        <v>3292800</v>
-      </c>
-      <c r="Z138" s="8" t="n"/>
-      <c r="AA138" s="8" t="n"/>
     </row>
     <row r="139">
       <c r="A139" s="7" t="n">
@@ -9418,11 +8793,6 @@
         <v>263424</v>
       </c>
       <c r="X139" s="8" t="n"/>
-      <c r="Y139" s="8" t="n"/>
-      <c r="Z139" s="8" t="n">
-        <v>263424</v>
-      </c>
-      <c r="AA139" s="8" t="n"/>
     </row>
     <row r="140">
       <c r="A140" s="7" t="n">
@@ -9475,11 +8845,6 @@
       <c r="V140" s="8" t="n"/>
       <c r="W140" s="8" t="n"/>
       <c r="X140" s="8" t="n">
-        <v>131712</v>
-      </c>
-      <c r="Y140" s="8" t="n"/>
-      <c r="Z140" s="8" t="n"/>
-      <c r="AA140" s="8" t="n">
         <v>131712</v>
       </c>
     </row>
@@ -9532,11 +8897,6 @@
         <v>131040</v>
       </c>
       <c r="X141" s="8" t="n"/>
-      <c r="Y141" s="8" t="n"/>
-      <c r="Z141" s="8" t="n">
-        <v>131040</v>
-      </c>
-      <c r="AA141" s="8" t="n"/>
     </row>
     <row r="142">
       <c r="A142" s="7" t="n">
@@ -9585,9 +8945,6 @@
       <c r="V142" s="8" t="n"/>
       <c r="W142" s="8" t="n"/>
       <c r="X142" s="8" t="n"/>
-      <c r="Y142" s="8" t="n"/>
-      <c r="Z142" s="8" t="n"/>
-      <c r="AA142" s="8" t="n"/>
     </row>
     <row r="143">
       <c r="A143" s="7" t="n">
@@ -9656,11 +9013,6 @@
       </c>
       <c r="W143" s="8" t="n"/>
       <c r="X143" s="8" t="n"/>
-      <c r="Y143" s="8" t="n">
-        <v>18844</v>
-      </c>
-      <c r="Z143" s="8" t="n"/>
-      <c r="AA143" s="8" t="n"/>
     </row>
     <row r="144">
       <c r="A144" s="7" t="n">
@@ -9729,11 +9081,6 @@
       </c>
       <c r="W144" s="8" t="n"/>
       <c r="X144" s="8" t="n"/>
-      <c r="Y144" s="8" t="n">
-        <v>19488</v>
-      </c>
-      <c r="Z144" s="8" t="n"/>
-      <c r="AA144" s="8" t="n"/>
     </row>
     <row r="145">
       <c r="A145" s="7" t="n">
@@ -9792,9 +9139,6 @@
       <c r="V145" s="8" t="n"/>
       <c r="W145" s="8" t="n"/>
       <c r="X145" s="8" t="n"/>
-      <c r="Y145" s="8" t="n"/>
-      <c r="Z145" s="8" t="n"/>
-      <c r="AA145" s="8" t="n"/>
     </row>
     <row r="146">
       <c r="A146" s="7" t="n">
@@ -9863,11 +9207,6 @@
       </c>
       <c r="W146" s="8" t="n"/>
       <c r="X146" s="8" t="n"/>
-      <c r="Y146" s="8" t="n">
-        <v>14751744</v>
-      </c>
-      <c r="Z146" s="8" t="n"/>
-      <c r="AA146" s="8" t="n"/>
     </row>
     <row r="147">
       <c r="A147" s="7" t="n">
@@ -9924,11 +9263,6 @@
         <v>43904</v>
       </c>
       <c r="X147" s="8" t="n"/>
-      <c r="Y147" s="8" t="n"/>
-      <c r="Z147" s="8" t="n">
-        <v>43904</v>
-      </c>
-      <c r="AA147" s="8" t="n"/>
     </row>
     <row r="148">
       <c r="A148" s="7" t="n">
@@ -9981,9 +9315,6 @@
       <c r="V148" s="8" t="n"/>
       <c r="W148" s="8" t="n"/>
       <c r="X148" s="8" t="n"/>
-      <c r="Y148" s="8" t="n"/>
-      <c r="Z148" s="8" t="n"/>
-      <c r="AA148" s="8" t="n"/>
     </row>
     <row r="149">
       <c r="A149" s="7" t="n">
@@ -10044,11 +9375,6 @@
         <v>21952</v>
       </c>
       <c r="X149" s="8" t="n"/>
-      <c r="Y149" s="8" t="n"/>
-      <c r="Z149" s="8" t="n">
-        <v>21952</v>
-      </c>
-      <c r="AA149" s="8" t="n"/>
     </row>
     <row r="150">
       <c r="A150" s="7" t="n">
@@ -10117,11 +9443,6 @@
       </c>
       <c r="W150" s="8" t="n"/>
       <c r="X150" s="8" t="n"/>
-      <c r="Y150" s="8" t="n">
-        <v>14751744</v>
-      </c>
-      <c r="Z150" s="8" t="n"/>
-      <c r="AA150" s="8" t="n"/>
     </row>
     <row r="151">
       <c r="A151" s="7" t="n">
@@ -10178,11 +9499,6 @@
         <v>263424</v>
       </c>
       <c r="X151" s="8" t="n"/>
-      <c r="Y151" s="8" t="n"/>
-      <c r="Z151" s="8" t="n">
-        <v>263424</v>
-      </c>
-      <c r="AA151" s="8" t="n"/>
     </row>
     <row r="152">
       <c r="A152" s="7" t="n">
@@ -10237,11 +9553,6 @@
       <c r="X152" s="8" t="n">
         <v>131712</v>
       </c>
-      <c r="Y152" s="8" t="n"/>
-      <c r="Z152" s="8" t="n"/>
-      <c r="AA152" s="8" t="n">
-        <v>131712</v>
-      </c>
     </row>
     <row r="153">
       <c r="A153" s="7" t="n">
@@ -10310,11 +9621,6 @@
       </c>
       <c r="W153" s="8" t="n"/>
       <c r="X153" s="8" t="n"/>
-      <c r="Y153" s="8" t="n">
-        <v>3292800</v>
-      </c>
-      <c r="Z153" s="8" t="n"/>
-      <c r="AA153" s="8" t="n"/>
     </row>
     <row r="154">
       <c r="A154" s="7" t="n">
@@ -10371,11 +9677,6 @@
         <v>263424</v>
       </c>
       <c r="X154" s="8" t="n"/>
-      <c r="Y154" s="8" t="n"/>
-      <c r="Z154" s="8" t="n">
-        <v>263424</v>
-      </c>
-      <c r="AA154" s="8" t="n"/>
     </row>
     <row r="155">
       <c r="A155" s="7" t="n">
@@ -10428,11 +9729,6 @@
       <c r="V155" s="8" t="n"/>
       <c r="W155" s="8" t="n"/>
       <c r="X155" s="8" t="n">
-        <v>131712</v>
-      </c>
-      <c r="Y155" s="8" t="n"/>
-      <c r="Z155" s="8" t="n"/>
-      <c r="AA155" s="8" t="n">
         <v>131712</v>
       </c>
     </row>
@@ -10485,11 +9781,6 @@
         <v>131040</v>
       </c>
       <c r="X156" s="8" t="n"/>
-      <c r="Y156" s="8" t="n"/>
-      <c r="Z156" s="8" t="n">
-        <v>131040</v>
-      </c>
-      <c r="AA156" s="8" t="n"/>
     </row>
     <row r="157">
       <c r="A157" s="7" t="n">
@@ -10538,9 +9829,6 @@
       <c r="V157" s="8" t="n"/>
       <c r="W157" s="8" t="n"/>
       <c r="X157" s="8" t="n"/>
-      <c r="Y157" s="8" t="n"/>
-      <c r="Z157" s="8" t="n"/>
-      <c r="AA157" s="8" t="n"/>
     </row>
     <row r="158">
       <c r="A158" s="7" t="n">
@@ -10609,11 +9897,6 @@
       </c>
       <c r="W158" s="8" t="n"/>
       <c r="X158" s="8" t="n"/>
-      <c r="Y158" s="8" t="n">
-        <v>18844</v>
-      </c>
-      <c r="Z158" s="8" t="n"/>
-      <c r="AA158" s="8" t="n"/>
     </row>
     <row r="159">
       <c r="A159" s="7" t="n">
@@ -10682,11 +9965,6 @@
       </c>
       <c r="W159" s="8" t="n"/>
       <c r="X159" s="8" t="n"/>
-      <c r="Y159" s="8" t="n">
-        <v>19488</v>
-      </c>
-      <c r="Z159" s="8" t="n"/>
-      <c r="AA159" s="8" t="n"/>
     </row>
     <row r="160">
       <c r="A160" s="7" t="n">
@@ -10745,9 +10023,6 @@
       <c r="V160" s="8" t="n"/>
       <c r="W160" s="8" t="n"/>
       <c r="X160" s="8" t="n"/>
-      <c r="Y160" s="8" t="n"/>
-      <c r="Z160" s="8" t="n"/>
-      <c r="AA160" s="8" t="n"/>
     </row>
     <row r="161">
       <c r="A161" s="7" t="n">
@@ -10816,11 +10091,6 @@
       </c>
       <c r="W161" s="8" t="n"/>
       <c r="X161" s="8" t="n"/>
-      <c r="Y161" s="8" t="n">
-        <v>14751744</v>
-      </c>
-      <c r="Z161" s="8" t="n"/>
-      <c r="AA161" s="8" t="n"/>
     </row>
     <row r="162">
       <c r="A162" s="7" t="n">
@@ -10877,11 +10147,6 @@
         <v>43904</v>
       </c>
       <c r="X162" s="8" t="n"/>
-      <c r="Y162" s="8" t="n"/>
-      <c r="Z162" s="8" t="n">
-        <v>43904</v>
-      </c>
-      <c r="AA162" s="8" t="n"/>
     </row>
     <row r="163">
       <c r="A163" s="7" t="n">
@@ -10934,9 +10199,6 @@
       <c r="V163" s="8" t="n"/>
       <c r="W163" s="8" t="n"/>
       <c r="X163" s="8" t="n"/>
-      <c r="Y163" s="8" t="n"/>
-      <c r="Z163" s="8" t="n"/>
-      <c r="AA163" s="8" t="n"/>
     </row>
     <row r="164">
       <c r="A164" s="7" t="n">
@@ -10997,11 +10259,6 @@
         <v>21952</v>
       </c>
       <c r="X164" s="8" t="n"/>
-      <c r="Y164" s="8" t="n"/>
-      <c r="Z164" s="8" t="n">
-        <v>21952</v>
-      </c>
-      <c r="AA164" s="8" t="n"/>
     </row>
     <row r="165">
       <c r="A165" s="7" t="n">
@@ -11070,11 +10327,6 @@
       </c>
       <c r="W165" s="8" t="n"/>
       <c r="X165" s="8" t="n"/>
-      <c r="Y165" s="8" t="n">
-        <v>14751744</v>
-      </c>
-      <c r="Z165" s="8" t="n"/>
-      <c r="AA165" s="8" t="n"/>
     </row>
     <row r="166">
       <c r="A166" s="7" t="n">
@@ -11131,11 +10383,6 @@
         <v>263424</v>
       </c>
       <c r="X166" s="8" t="n"/>
-      <c r="Y166" s="8" t="n"/>
-      <c r="Z166" s="8" t="n">
-        <v>263424</v>
-      </c>
-      <c r="AA166" s="8" t="n"/>
     </row>
     <row r="167">
       <c r="A167" s="7" t="n">
@@ -11190,11 +10437,6 @@
       <c r="X167" s="8" t="n">
         <v>131712</v>
       </c>
-      <c r="Y167" s="8" t="n"/>
-      <c r="Z167" s="8" t="n"/>
-      <c r="AA167" s="8" t="n">
-        <v>131712</v>
-      </c>
     </row>
     <row r="168">
       <c r="A168" s="7" t="n">
@@ -11247,9 +10489,6 @@
       <c r="V168" s="8" t="n"/>
       <c r="W168" s="8" t="n"/>
       <c r="X168" s="8" t="n"/>
-      <c r="Y168" s="8" t="n"/>
-      <c r="Z168" s="8" t="n"/>
-      <c r="AA168" s="8" t="n"/>
     </row>
     <row r="169">
       <c r="A169" s="7" t="n">
@@ -11318,11 +10557,6 @@
       </c>
       <c r="W169" s="8" t="n"/>
       <c r="X169" s="8" t="n"/>
-      <c r="Y169" s="8" t="n">
-        <v>823200</v>
-      </c>
-      <c r="Z169" s="8" t="n"/>
-      <c r="AA169" s="8" t="n"/>
     </row>
     <row r="170">
       <c r="A170" s="7" t="n">
@@ -11379,11 +10613,6 @@
         <v>65856</v>
       </c>
       <c r="X170" s="8" t="n"/>
-      <c r="Y170" s="8" t="n"/>
-      <c r="Z170" s="8" t="n">
-        <v>65856</v>
-      </c>
-      <c r="AA170" s="8" t="n"/>
     </row>
     <row r="171">
       <c r="A171" s="7" t="n">
@@ -11436,11 +10665,6 @@
       <c r="V171" s="8" t="n"/>
       <c r="W171" s="8" t="n"/>
       <c r="X171" s="8" t="n">
-        <v>32928</v>
-      </c>
-      <c r="Y171" s="8" t="n"/>
-      <c r="Z171" s="8" t="n"/>
-      <c r="AA171" s="8" t="n">
         <v>32928</v>
       </c>
     </row>
@@ -11493,11 +10717,6 @@
         <v>32256</v>
       </c>
       <c r="X172" s="8" t="n"/>
-      <c r="Y172" s="8" t="n"/>
-      <c r="Z172" s="8" t="n">
-        <v>32256</v>
-      </c>
-      <c r="AA172" s="8" t="n"/>
     </row>
     <row r="173">
       <c r="A173" s="7" t="n">
@@ -11546,9 +10765,6 @@
       <c r="V173" s="8" t="n"/>
       <c r="W173" s="8" t="n"/>
       <c r="X173" s="8" t="n"/>
-      <c r="Y173" s="8" t="n"/>
-      <c r="Z173" s="8" t="n"/>
-      <c r="AA173" s="8" t="n"/>
     </row>
     <row r="174">
       <c r="A174" s="7" t="n">
@@ -11617,11 +10833,6 @@
       </c>
       <c r="W174" s="8" t="n"/>
       <c r="X174" s="8" t="n"/>
-      <c r="Y174" s="8" t="n">
-        <v>18844</v>
-      </c>
-      <c r="Z174" s="8" t="n"/>
-      <c r="AA174" s="8" t="n"/>
     </row>
     <row r="175">
       <c r="A175" s="7" t="n">
@@ -11690,11 +10901,6 @@
       </c>
       <c r="W175" s="8" t="n"/>
       <c r="X175" s="8" t="n"/>
-      <c r="Y175" s="8" t="n">
-        <v>19488</v>
-      </c>
-      <c r="Z175" s="8" t="n"/>
-      <c r="AA175" s="8" t="n"/>
     </row>
     <row r="176">
       <c r="A176" s="7" t="n">
@@ -11753,9 +10959,6 @@
       <c r="V176" s="8" t="n"/>
       <c r="W176" s="8" t="n"/>
       <c r="X176" s="8" t="n"/>
-      <c r="Y176" s="8" t="n"/>
-      <c r="Z176" s="8" t="n"/>
-      <c r="AA176" s="8" t="n"/>
     </row>
     <row r="177">
       <c r="A177" s="7" t="n">
@@ -11824,11 +11027,6 @@
       </c>
       <c r="W177" s="8" t="n"/>
       <c r="X177" s="8" t="n"/>
-      <c r="Y177" s="8" t="n">
-        <v>6322176</v>
-      </c>
-      <c r="Z177" s="8" t="n"/>
-      <c r="AA177" s="8" t="n"/>
     </row>
     <row r="178">
       <c r="A178" s="7" t="n">
@@ -11885,11 +11083,6 @@
         <v>18816</v>
       </c>
       <c r="X178" s="8" t="n"/>
-      <c r="Y178" s="8" t="n"/>
-      <c r="Z178" s="8" t="n">
-        <v>18816</v>
-      </c>
-      <c r="AA178" s="8" t="n"/>
     </row>
     <row r="179">
       <c r="A179" s="7" t="n">
@@ -11958,11 +11151,6 @@
       </c>
       <c r="W179" s="8" t="n"/>
       <c r="X179" s="8" t="n"/>
-      <c r="Y179" s="8" t="n">
-        <v>10838016</v>
-      </c>
-      <c r="Z179" s="8" t="n"/>
-      <c r="AA179" s="8" t="n"/>
     </row>
     <row r="180">
       <c r="A180" s="7" t="n">
@@ -12019,11 +11207,6 @@
         <v>112896</v>
       </c>
       <c r="X180" s="8" t="n"/>
-      <c r="Y180" s="8" t="n"/>
-      <c r="Z180" s="8" t="n">
-        <v>112896</v>
-      </c>
-      <c r="AA180" s="8" t="n"/>
     </row>
     <row r="181">
       <c r="A181" s="7" t="n">
@@ -12078,11 +11261,6 @@
       <c r="X181" s="8" t="n">
         <v>56448</v>
       </c>
-      <c r="Y181" s="8" t="n"/>
-      <c r="Z181" s="8" t="n"/>
-      <c r="AA181" s="8" t="n">
-        <v>56448</v>
-      </c>
     </row>
     <row r="182">
       <c r="A182" s="7" t="n">
@@ -12151,11 +11329,6 @@
       </c>
       <c r="W182" s="8" t="n"/>
       <c r="X182" s="8" t="n"/>
-      <c r="Y182" s="8" t="n">
-        <v>1411200</v>
-      </c>
-      <c r="Z182" s="8" t="n"/>
-      <c r="AA182" s="8" t="n"/>
     </row>
     <row r="183">
       <c r="A183" s="7" t="n">
@@ -12212,11 +11385,6 @@
         <v>112896</v>
       </c>
       <c r="X183" s="8" t="n"/>
-      <c r="Y183" s="8" t="n"/>
-      <c r="Z183" s="8" t="n">
-        <v>112896</v>
-      </c>
-      <c r="AA183" s="8" t="n"/>
     </row>
     <row r="184">
       <c r="A184" s="7" t="n">
@@ -12269,11 +11437,6 @@
       <c r="V184" s="8" t="n"/>
       <c r="W184" s="8" t="n"/>
       <c r="X184" s="8" t="n">
-        <v>56448</v>
-      </c>
-      <c r="Y184" s="8" t="n"/>
-      <c r="Z184" s="8" t="n"/>
-      <c r="AA184" s="8" t="n">
         <v>56448</v>
       </c>
     </row>
@@ -12326,11 +11489,6 @@
         <v>55296</v>
       </c>
       <c r="X185" s="8" t="n"/>
-      <c r="Y185" s="8" t="n"/>
-      <c r="Z185" s="8" t="n">
-        <v>55296</v>
-      </c>
-      <c r="AA185" s="8" t="n"/>
     </row>
     <row r="186">
       <c r="A186" s="7" t="n">
@@ -12379,9 +11537,6 @@
       <c r="V186" s="8" t="n"/>
       <c r="W186" s="8" t="n"/>
       <c r="X186" s="8" t="n"/>
-      <c r="Y186" s="8" t="n"/>
-      <c r="Z186" s="8" t="n"/>
-      <c r="AA186" s="8" t="n"/>
     </row>
     <row r="187">
       <c r="A187" s="7" t="n">
@@ -12450,11 +11605,6 @@
       </c>
       <c r="W187" s="8" t="n"/>
       <c r="X187" s="8" t="n"/>
-      <c r="Y187" s="8" t="n">
-        <v>55344</v>
-      </c>
-      <c r="Z187" s="8" t="n"/>
-      <c r="AA187" s="8" t="n"/>
     </row>
     <row r="188">
       <c r="A188" s="7" t="n">
@@ -12523,11 +11673,6 @@
       </c>
       <c r="W188" s="8" t="n"/>
       <c r="X188" s="8" t="n"/>
-      <c r="Y188" s="8" t="n">
-        <v>56448</v>
-      </c>
-      <c r="Z188" s="8" t="n"/>
-      <c r="AA188" s="8" t="n"/>
     </row>
     <row r="189">
       <c r="A189" s="7" t="n">
@@ -12586,9 +11731,6 @@
       <c r="V189" s="8" t="n"/>
       <c r="W189" s="8" t="n"/>
       <c r="X189" s="8" t="n"/>
-      <c r="Y189" s="8" t="n"/>
-      <c r="Z189" s="8" t="n"/>
-      <c r="AA189" s="8" t="n"/>
     </row>
     <row r="190">
       <c r="A190" s="7" t="n">
@@ -12657,11 +11799,6 @@
       </c>
       <c r="W190" s="8" t="n"/>
       <c r="X190" s="8" t="n"/>
-      <c r="Y190" s="8" t="n">
-        <v>10838016</v>
-      </c>
-      <c r="Z190" s="8" t="n"/>
-      <c r="AA190" s="8" t="n"/>
     </row>
     <row r="191">
       <c r="A191" s="7" t="n">
@@ -12718,11 +11855,6 @@
         <v>18816</v>
       </c>
       <c r="X191" s="8" t="n"/>
-      <c r="Y191" s="8" t="n"/>
-      <c r="Z191" s="8" t="n">
-        <v>18816</v>
-      </c>
-      <c r="AA191" s="8" t="n"/>
     </row>
     <row r="192">
       <c r="A192" s="7" t="n">
@@ -12775,9 +11907,6 @@
       <c r="V192" s="8" t="n"/>
       <c r="W192" s="8" t="n"/>
       <c r="X192" s="8" t="n"/>
-      <c r="Y192" s="8" t="n"/>
-      <c r="Z192" s="8" t="n"/>
-      <c r="AA192" s="8" t="n"/>
     </row>
     <row r="193">
       <c r="A193" s="7" t="n">
@@ -12838,11 +11967,6 @@
         <v>9408</v>
       </c>
       <c r="X193" s="8" t="n"/>
-      <c r="Y193" s="8" t="n"/>
-      <c r="Z193" s="8" t="n">
-        <v>9408</v>
-      </c>
-      <c r="AA193" s="8" t="n"/>
     </row>
     <row r="194">
       <c r="A194" s="7" t="n">
@@ -12911,11 +12035,6 @@
       </c>
       <c r="W194" s="8" t="n"/>
       <c r="X194" s="8" t="n"/>
-      <c r="Y194" s="8" t="n">
-        <v>10838016</v>
-      </c>
-      <c r="Z194" s="8" t="n"/>
-      <c r="AA194" s="8" t="n"/>
     </row>
     <row r="195">
       <c r="A195" s="7" t="n">
@@ -12972,11 +12091,6 @@
         <v>112896</v>
       </c>
       <c r="X195" s="8" t="n"/>
-      <c r="Y195" s="8" t="n"/>
-      <c r="Z195" s="8" t="n">
-        <v>112896</v>
-      </c>
-      <c r="AA195" s="8" t="n"/>
     </row>
     <row r="196">
       <c r="A196" s="7" t="n">
@@ -13031,11 +12145,6 @@
       <c r="X196" s="8" t="n">
         <v>56448</v>
       </c>
-      <c r="Y196" s="8" t="n"/>
-      <c r="Z196" s="8" t="n"/>
-      <c r="AA196" s="8" t="n">
-        <v>56448</v>
-      </c>
     </row>
     <row r="197">
       <c r="A197" s="7" t="n">
@@ -13104,11 +12213,6 @@
       </c>
       <c r="W197" s="8" t="n"/>
       <c r="X197" s="8" t="n"/>
-      <c r="Y197" s="8" t="n">
-        <v>1411200</v>
-      </c>
-      <c r="Z197" s="8" t="n"/>
-      <c r="AA197" s="8" t="n"/>
     </row>
     <row r="198">
       <c r="A198" s="7" t="n">
@@ -13165,11 +12269,6 @@
         <v>112896</v>
       </c>
       <c r="X198" s="8" t="n"/>
-      <c r="Y198" s="8" t="n"/>
-      <c r="Z198" s="8" t="n">
-        <v>112896</v>
-      </c>
-      <c r="AA198" s="8" t="n"/>
     </row>
     <row r="199">
       <c r="A199" s="7" t="n">
@@ -13222,11 +12321,6 @@
       <c r="V199" s="8" t="n"/>
       <c r="W199" s="8" t="n"/>
       <c r="X199" s="8" t="n">
-        <v>56448</v>
-      </c>
-      <c r="Y199" s="8" t="n"/>
-      <c r="Z199" s="8" t="n"/>
-      <c r="AA199" s="8" t="n">
         <v>56448</v>
       </c>
     </row>
@@ -13279,11 +12373,6 @@
         <v>55296</v>
       </c>
       <c r="X200" s="8" t="n"/>
-      <c r="Y200" s="8" t="n"/>
-      <c r="Z200" s="8" t="n">
-        <v>55296</v>
-      </c>
-      <c r="AA200" s="8" t="n"/>
     </row>
     <row r="201">
       <c r="A201" s="7" t="n">
@@ -13332,9 +12421,6 @@
       <c r="V201" s="8" t="n"/>
       <c r="W201" s="8" t="n"/>
       <c r="X201" s="8" t="n"/>
-      <c r="Y201" s="8" t="n"/>
-      <c r="Z201" s="8" t="n"/>
-      <c r="AA201" s="8" t="n"/>
     </row>
     <row r="202">
       <c r="A202" s="7" t="n">
@@ -13403,11 +12489,6 @@
       </c>
       <c r="W202" s="8" t="n"/>
       <c r="X202" s="8" t="n"/>
-      <c r="Y202" s="8" t="n">
-        <v>55344</v>
-      </c>
-      <c r="Z202" s="8" t="n"/>
-      <c r="AA202" s="8" t="n"/>
     </row>
     <row r="203">
       <c r="A203" s="7" t="n">
@@ -13476,11 +12557,6 @@
       </c>
       <c r="W203" s="8" t="n"/>
       <c r="X203" s="8" t="n"/>
-      <c r="Y203" s="8" t="n">
-        <v>56448</v>
-      </c>
-      <c r="Z203" s="8" t="n"/>
-      <c r="AA203" s="8" t="n"/>
     </row>
     <row r="204">
       <c r="A204" s="7" t="n">
@@ -13539,9 +12615,6 @@
       <c r="V204" s="8" t="n"/>
       <c r="W204" s="8" t="n"/>
       <c r="X204" s="8" t="n"/>
-      <c r="Y204" s="8" t="n"/>
-      <c r="Z204" s="8" t="n"/>
-      <c r="AA204" s="8" t="n"/>
     </row>
     <row r="205">
       <c r="A205" s="7" t="n">
@@ -13610,11 +12683,6 @@
       </c>
       <c r="W205" s="8" t="n"/>
       <c r="X205" s="8" t="n"/>
-      <c r="Y205" s="8" t="n">
-        <v>10838016</v>
-      </c>
-      <c r="Z205" s="8" t="n"/>
-      <c r="AA205" s="8" t="n"/>
     </row>
     <row r="206">
       <c r="A206" s="7" t="n">
@@ -13671,11 +12739,6 @@
         <v>18816</v>
       </c>
       <c r="X206" s="8" t="n"/>
-      <c r="Y206" s="8" t="n"/>
-      <c r="Z206" s="8" t="n">
-        <v>18816</v>
-      </c>
-      <c r="AA206" s="8" t="n"/>
     </row>
     <row r="207">
       <c r="A207" s="7" t="n">
@@ -13728,9 +12791,6 @@
       <c r="V207" s="8" t="n"/>
       <c r="W207" s="8" t="n"/>
       <c r="X207" s="8" t="n"/>
-      <c r="Y207" s="8" t="n"/>
-      <c r="Z207" s="8" t="n"/>
-      <c r="AA207" s="8" t="n"/>
     </row>
     <row r="208">
       <c r="A208" s="7" t="n">
@@ -13791,11 +12851,6 @@
         <v>9408</v>
       </c>
       <c r="X208" s="8" t="n"/>
-      <c r="Y208" s="8" t="n"/>
-      <c r="Z208" s="8" t="n">
-        <v>9408</v>
-      </c>
-      <c r="AA208" s="8" t="n"/>
     </row>
     <row r="209">
       <c r="A209" s="7" t="n">
@@ -13864,11 +12919,6 @@
       </c>
       <c r="W209" s="8" t="n"/>
       <c r="X209" s="8" t="n"/>
-      <c r="Y209" s="8" t="n">
-        <v>10838016</v>
-      </c>
-      <c r="Z209" s="8" t="n"/>
-      <c r="AA209" s="8" t="n"/>
     </row>
     <row r="210">
       <c r="A210" s="7" t="n">
@@ -13925,11 +12975,6 @@
         <v>112896</v>
       </c>
       <c r="X210" s="8" t="n"/>
-      <c r="Y210" s="8" t="n"/>
-      <c r="Z210" s="8" t="n">
-        <v>112896</v>
-      </c>
-      <c r="AA210" s="8" t="n"/>
     </row>
     <row r="211">
       <c r="A211" s="7" t="n">
@@ -13984,11 +13029,6 @@
       <c r="X211" s="8" t="n">
         <v>56448</v>
       </c>
-      <c r="Y211" s="8" t="n"/>
-      <c r="Z211" s="8" t="n"/>
-      <c r="AA211" s="8" t="n">
-        <v>56448</v>
-      </c>
     </row>
     <row r="212">
       <c r="A212" s="7" t="n">
@@ -14057,11 +13097,6 @@
       </c>
       <c r="W212" s="8" t="n"/>
       <c r="X212" s="8" t="n"/>
-      <c r="Y212" s="8" t="n">
-        <v>1411200</v>
-      </c>
-      <c r="Z212" s="8" t="n"/>
-      <c r="AA212" s="8" t="n"/>
     </row>
     <row r="213">
       <c r="A213" s="7" t="n">
@@ -14118,11 +13153,6 @@
         <v>112896</v>
       </c>
       <c r="X213" s="8" t="n"/>
-      <c r="Y213" s="8" t="n"/>
-      <c r="Z213" s="8" t="n">
-        <v>112896</v>
-      </c>
-      <c r="AA213" s="8" t="n"/>
     </row>
     <row r="214">
       <c r="A214" s="7" t="n">
@@ -14175,11 +13205,6 @@
       <c r="V214" s="8" t="n"/>
       <c r="W214" s="8" t="n"/>
       <c r="X214" s="8" t="n">
-        <v>56448</v>
-      </c>
-      <c r="Y214" s="8" t="n"/>
-      <c r="Z214" s="8" t="n"/>
-      <c r="AA214" s="8" t="n">
         <v>56448</v>
       </c>
     </row>
@@ -14232,11 +13257,6 @@
         <v>55296</v>
       </c>
       <c r="X215" s="8" t="n"/>
-      <c r="Y215" s="8" t="n"/>
-      <c r="Z215" s="8" t="n">
-        <v>55296</v>
-      </c>
-      <c r="AA215" s="8" t="n"/>
     </row>
     <row r="216">
       <c r="A216" s="7" t="n">
@@ -14285,9 +13305,6 @@
       <c r="V216" s="8" t="n"/>
       <c r="W216" s="8" t="n"/>
       <c r="X216" s="8" t="n"/>
-      <c r="Y216" s="8" t="n"/>
-      <c r="Z216" s="8" t="n"/>
-      <c r="AA216" s="8" t="n"/>
     </row>
     <row r="217">
       <c r="A217" s="7" t="n">
@@ -14356,11 +13373,6 @@
       </c>
       <c r="W217" s="8" t="n"/>
       <c r="X217" s="8" t="n"/>
-      <c r="Y217" s="8" t="n">
-        <v>55344</v>
-      </c>
-      <c r="Z217" s="8" t="n"/>
-      <c r="AA217" s="8" t="n"/>
     </row>
     <row r="218">
       <c r="A218" s="7" t="n">
@@ -14429,11 +13441,6 @@
       </c>
       <c r="W218" s="8" t="n"/>
       <c r="X218" s="8" t="n"/>
-      <c r="Y218" s="8" t="n">
-        <v>56448</v>
-      </c>
-      <c r="Z218" s="8" t="n"/>
-      <c r="AA218" s="8" t="n"/>
     </row>
     <row r="219">
       <c r="A219" s="7" t="n">
@@ -14492,9 +13499,6 @@
       <c r="V219" s="8" t="n"/>
       <c r="W219" s="8" t="n"/>
       <c r="X219" s="8" t="n"/>
-      <c r="Y219" s="8" t="n"/>
-      <c r="Z219" s="8" t="n"/>
-      <c r="AA219" s="8" t="n"/>
     </row>
     <row r="220">
       <c r="A220" s="7" t="n">
@@ -14563,11 +13567,6 @@
       </c>
       <c r="W220" s="8" t="n"/>
       <c r="X220" s="8" t="n"/>
-      <c r="Y220" s="8" t="n">
-        <v>10838016</v>
-      </c>
-      <c r="Z220" s="8" t="n"/>
-      <c r="AA220" s="8" t="n"/>
     </row>
     <row r="221">
       <c r="A221" s="7" t="n">
@@ -14624,11 +13623,6 @@
         <v>18816</v>
       </c>
       <c r="X221" s="8" t="n"/>
-      <c r="Y221" s="8" t="n"/>
-      <c r="Z221" s="8" t="n">
-        <v>18816</v>
-      </c>
-      <c r="AA221" s="8" t="n"/>
     </row>
     <row r="222">
       <c r="A222" s="7" t="n">
@@ -14681,9 +13675,6 @@
       <c r="V222" s="8" t="n"/>
       <c r="W222" s="8" t="n"/>
       <c r="X222" s="8" t="n"/>
-      <c r="Y222" s="8" t="n"/>
-      <c r="Z222" s="8" t="n"/>
-      <c r="AA222" s="8" t="n"/>
     </row>
     <row r="223">
       <c r="A223" s="7" t="n">
@@ -14744,11 +13735,6 @@
         <v>9408</v>
       </c>
       <c r="X223" s="8" t="n"/>
-      <c r="Y223" s="8" t="n"/>
-      <c r="Z223" s="8" t="n">
-        <v>9408</v>
-      </c>
-      <c r="AA223" s="8" t="n"/>
     </row>
     <row r="224">
       <c r="A224" s="7" t="n">
@@ -14817,11 +13803,6 @@
       </c>
       <c r="W224" s="8" t="n"/>
       <c r="X224" s="8" t="n"/>
-      <c r="Y224" s="8" t="n">
-        <v>10838016</v>
-      </c>
-      <c r="Z224" s="8" t="n"/>
-      <c r="AA224" s="8" t="n"/>
     </row>
     <row r="225">
       <c r="A225" s="7" t="n">
@@ -14878,11 +13859,6 @@
         <v>112896</v>
       </c>
       <c r="X225" s="8" t="n"/>
-      <c r="Y225" s="8" t="n"/>
-      <c r="Z225" s="8" t="n">
-        <v>112896</v>
-      </c>
-      <c r="AA225" s="8" t="n"/>
     </row>
     <row r="226">
       <c r="A226" s="7" t="n">
@@ -14937,11 +13913,6 @@
       <c r="X226" s="8" t="n">
         <v>56448</v>
       </c>
-      <c r="Y226" s="8" t="n"/>
-      <c r="Z226" s="8" t="n"/>
-      <c r="AA226" s="8" t="n">
-        <v>56448</v>
-      </c>
     </row>
     <row r="227">
       <c r="A227" s="7" t="n">
@@ -15010,11 +13981,6 @@
       </c>
       <c r="W227" s="8" t="n"/>
       <c r="X227" s="8" t="n"/>
-      <c r="Y227" s="8" t="n">
-        <v>508032</v>
-      </c>
-      <c r="Z227" s="8" t="n"/>
-      <c r="AA227" s="8" t="n"/>
     </row>
     <row r="228">
       <c r="A228" s="7" t="n">
@@ -15071,11 +14037,6 @@
         <v>112896</v>
       </c>
       <c r="X228" s="8" t="n"/>
-      <c r="Y228" s="8" t="n"/>
-      <c r="Z228" s="8" t="n">
-        <v>112896</v>
-      </c>
-      <c r="AA228" s="8" t="n"/>
     </row>
     <row r="229">
       <c r="A229" s="7" t="n">
@@ -15128,11 +14089,6 @@
       <c r="V229" s="8" t="n"/>
       <c r="W229" s="8" t="n"/>
       <c r="X229" s="8" t="n">
-        <v>56448</v>
-      </c>
-      <c r="Y229" s="8" t="n"/>
-      <c r="Z229" s="8" t="n"/>
-      <c r="AA229" s="8" t="n">
         <v>56448</v>
       </c>
     </row>
@@ -15185,11 +14141,6 @@
         <v>55296</v>
       </c>
       <c r="X230" s="8" t="n"/>
-      <c r="Y230" s="8" t="n"/>
-      <c r="Z230" s="8" t="n">
-        <v>55296</v>
-      </c>
-      <c r="AA230" s="8" t="n"/>
     </row>
     <row r="231">
       <c r="A231" s="7" t="n">
@@ -15238,9 +14189,6 @@
       <c r="V231" s="8" t="n"/>
       <c r="W231" s="8" t="n"/>
       <c r="X231" s="8" t="n"/>
-      <c r="Y231" s="8" t="n"/>
-      <c r="Z231" s="8" t="n"/>
-      <c r="AA231" s="8" t="n"/>
     </row>
     <row r="232">
       <c r="A232" s="7" t="n">
@@ -15309,11 +14257,6 @@
       </c>
       <c r="W232" s="8" t="n"/>
       <c r="X232" s="8" t="n"/>
-      <c r="Y232" s="8" t="n">
-        <v>55344</v>
-      </c>
-      <c r="Z232" s="8" t="n"/>
-      <c r="AA232" s="8" t="n"/>
     </row>
     <row r="233">
       <c r="A233" s="7" t="n">
@@ -15382,11 +14325,6 @@
       </c>
       <c r="W233" s="8" t="n"/>
       <c r="X233" s="8" t="n"/>
-      <c r="Y233" s="8" t="n">
-        <v>56448</v>
-      </c>
-      <c r="Z233" s="8" t="n"/>
-      <c r="AA233" s="8" t="n"/>
     </row>
     <row r="234">
       <c r="A234" s="7" t="n">
@@ -15445,9 +14383,6 @@
       <c r="V234" s="8" t="n"/>
       <c r="W234" s="8" t="n"/>
       <c r="X234" s="8" t="n"/>
-      <c r="Y234" s="8" t="n"/>
-      <c r="Z234" s="8" t="n"/>
-      <c r="AA234" s="8" t="n"/>
     </row>
     <row r="235">
       <c r="A235" s="7" t="n">
@@ -15516,11 +14451,6 @@
       </c>
       <c r="W235" s="8" t="n"/>
       <c r="X235" s="8" t="n"/>
-      <c r="Y235" s="8" t="n">
-        <v>18063360</v>
-      </c>
-      <c r="Z235" s="8" t="n"/>
-      <c r="AA235" s="8" t="n"/>
     </row>
     <row r="236">
       <c r="A236" s="7" t="n">
@@ -15577,11 +14507,6 @@
         <v>31360</v>
       </c>
       <c r="X236" s="8" t="n"/>
-      <c r="Y236" s="8" t="n"/>
-      <c r="Z236" s="8" t="n">
-        <v>31360</v>
-      </c>
-      <c r="AA236" s="8" t="n"/>
     </row>
     <row r="237">
       <c r="A237" s="7" t="n">
@@ -15650,11 +14575,6 @@
       </c>
       <c r="W237" s="8" t="n"/>
       <c r="X237" s="8" t="n"/>
-      <c r="Y237" s="8" t="n">
-        <v>20070400</v>
-      </c>
-      <c r="Z237" s="8" t="n"/>
-      <c r="AA237" s="8" t="n"/>
     </row>
     <row r="238">
       <c r="A238" s="7" t="n">
@@ -15711,11 +14631,6 @@
         <v>125440</v>
       </c>
       <c r="X238" s="8" t="n"/>
-      <c r="Y238" s="8" t="n"/>
-      <c r="Z238" s="8" t="n">
-        <v>125440</v>
-      </c>
-      <c r="AA238" s="8" t="n"/>
     </row>
     <row r="239">
       <c r="A239" s="7" t="n">
@@ -15768,11 +14683,6 @@
       <c r="V239" s="8" t="n"/>
       <c r="W239" s="8" t="n"/>
       <c r="X239" s="8" t="n">
-        <v>62720</v>
-      </c>
-      <c r="Y239" s="8" t="n"/>
-      <c r="Z239" s="8" t="n"/>
-      <c r="AA239" s="8" t="n">
         <v>62720</v>
       </c>
     </row>
@@ -15825,11 +14735,6 @@
         <v>61440</v>
       </c>
       <c r="X240" s="8" t="n"/>
-      <c r="Y240" s="8" t="n"/>
-      <c r="Z240" s="8" t="n">
-        <v>61440</v>
-      </c>
-      <c r="AA240" s="8" t="n"/>
     </row>
     <row r="241">
       <c r="A241" s="7" t="n">
@@ -15874,9 +14779,6 @@
       <c r="V241" s="8" t="n"/>
       <c r="W241" s="8" t="n"/>
       <c r="X241" s="8" t="n"/>
-      <c r="Y241" s="8" t="n"/>
-      <c r="Z241" s="8" t="n"/>
-      <c r="AA241" s="8" t="n"/>
     </row>
     <row r="242">
       <c r="A242" s="7" t="n">
@@ -15927,16 +14829,9 @@
       <c r="X242" s="8" t="n">
         <v>1280</v>
       </c>
-      <c r="Y242" s="8" t="n">
-        <v>1281000</v>
-      </c>
-      <c r="Z242" s="8" t="n"/>
-      <c r="AA242" s="8" t="n">
-        <v>1280</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>
@@ -15946,7 +14841,6 @@
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="V1:X1"/>
-    <mergeCell ref="Y1:AA1"/>
   </mergeCells>
   <conditionalFormatting sqref="T1:T242">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
@@ -15963,12 +14857,7 @@
       <formula>20070400</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y1:Y242">
-    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3" stopIfTrue="1">
-      <formula>20070400</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>